<commit_message>
Toutes les clés et pivots placées définitivement + mécanismes kinematics + tableau de correspondance Clé - Mécanisme
</commit_message>
<xml_diff>
--- a/activation_cles.xlsx
+++ b/activation_cles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Documents\ECL\Electifs\PLM Maquette numerique\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587DA713-7BCE-4CD3-B0CF-49B9CABD30F9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A865D97E-9A29-449B-8676-617E6FC54B46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{F09C0DAC-A25C-4A53-8295-137620DF1250}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Mi3</t>
   </si>
@@ -153,13 +153,7 @@
     <t>Cle_inf_3_fa</t>
   </si>
   <si>
-    <t>Cle_inf_6_mi_g</t>
-  </si>
-  <si>
     <t>Cle_inf_4_mi_d</t>
-  </si>
-  <si>
-    <t>Cle_inf_7_fadiese_g</t>
   </si>
   <si>
     <t>Cle_inf_5_fadiese_d</t>
@@ -668,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A9C269-1E13-45B8-9E0A-29C53F2C95DD}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,21 +682,20 @@
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>35</v>
@@ -734,17 +727,11 @@
       <c r="N1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -787,17 +774,11 @@
       <c r="N2" s="12">
         <v>1</v>
       </c>
-      <c r="O2" s="12">
-        <v>1</v>
-      </c>
-      <c r="P2" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -840,17 +821,11 @@
       <c r="N3" s="8">
         <v>0</v>
       </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -893,17 +868,11 @@
       <c r="N4" s="8">
         <v>0</v>
       </c>
-      <c r="O4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -946,17 +915,11 @@
       <c r="N5" s="8">
         <v>0</v>
       </c>
-      <c r="O5" s="8">
-        <v>0</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -999,17 +962,11 @@
       <c r="N6" s="8">
         <v>0</v>
       </c>
-      <c r="O6" s="8">
-        <v>0</v>
-      </c>
-      <c r="P6" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1052,17 +1009,11 @@
       <c r="N7" s="8">
         <v>0</v>
       </c>
-      <c r="O7" s="8">
-        <v>0</v>
-      </c>
-      <c r="P7" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -1105,17 +1056,11 @@
       <c r="N8" s="8">
         <v>0</v>
       </c>
-      <c r="O8" s="8">
-        <v>0</v>
-      </c>
-      <c r="P8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1158,17 +1103,11 @@
       <c r="N9" s="8">
         <v>0</v>
       </c>
-      <c r="O9" s="8">
-        <v>0</v>
-      </c>
-      <c r="P9" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1211,17 +1150,11 @@
       <c r="N10" s="8">
         <v>0</v>
       </c>
-      <c r="O10" s="8">
-        <v>0</v>
-      </c>
-      <c r="P10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1264,17 +1197,11 @@
       <c r="N11" s="8">
         <v>0</v>
       </c>
-      <c r="O11" s="8">
-        <v>0</v>
-      </c>
-      <c r="P11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -1317,17 +1244,11 @@
       <c r="N12" s="8">
         <v>0</v>
       </c>
-      <c r="O12" s="8">
-        <v>0</v>
-      </c>
-      <c r="P12" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -1370,17 +1291,11 @@
       <c r="N13" s="8">
         <v>0</v>
       </c>
-      <c r="O13" s="8">
-        <v>0</v>
-      </c>
-      <c r="P13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -1423,17 +1338,11 @@
       <c r="N14" s="8">
         <v>0</v>
       </c>
-      <c r="O14" s="8">
-        <v>0</v>
-      </c>
-      <c r="P14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1476,17 +1385,11 @@
       <c r="N15" s="8">
         <v>0</v>
       </c>
-      <c r="O15" s="8">
-        <v>0</v>
-      </c>
-      <c r="P15" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -1529,17 +1432,11 @@
       <c r="N16" s="8">
         <v>0</v>
       </c>
-      <c r="O16" s="8">
-        <v>0</v>
-      </c>
-      <c r="P16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -1582,17 +1479,11 @@
       <c r="N17" s="8">
         <v>0</v>
       </c>
-      <c r="O17" s="8">
-        <v>0</v>
-      </c>
-      <c r="P17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -1635,17 +1526,11 @@
       <c r="N18" s="8">
         <v>0</v>
       </c>
-      <c r="O18" s="8">
-        <v>0</v>
-      </c>
-      <c r="P18" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -1688,17 +1573,11 @@
       <c r="N19" s="8">
         <v>0</v>
       </c>
-      <c r="O19" s="8">
-        <v>0</v>
-      </c>
-      <c r="P19" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1741,17 +1620,11 @@
       <c r="N20" s="8">
         <v>0</v>
       </c>
-      <c r="O20" s="8">
-        <v>0</v>
-      </c>
-      <c r="P20" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1794,17 +1667,11 @@
       <c r="N21" s="12">
         <v>1</v>
       </c>
-      <c r="O21" s="12">
-        <v>1</v>
-      </c>
-      <c r="P21" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
@@ -1847,17 +1714,11 @@
       <c r="N22" s="8">
         <v>0</v>
       </c>
-      <c r="O22" s="8">
-        <v>0</v>
-      </c>
-      <c r="P22" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
@@ -1900,17 +1761,11 @@
       <c r="N23" s="8">
         <v>0</v>
       </c>
-      <c r="O23" s="8">
-        <v>0</v>
-      </c>
-      <c r="P23" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O23" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -1953,17 +1808,11 @@
       <c r="N24" s="8">
         <v>0</v>
       </c>
-      <c r="O24" s="8">
-        <v>0</v>
-      </c>
-      <c r="P24" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
@@ -2006,17 +1855,11 @@
       <c r="N25" s="8">
         <v>0</v>
       </c>
-      <c r="O25" s="8">
-        <v>0</v>
-      </c>
-      <c r="P25" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
@@ -2059,17 +1902,11 @@
       <c r="N26" s="8">
         <v>0</v>
       </c>
-      <c r="O26" s="8">
-        <v>0</v>
-      </c>
-      <c r="P26" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -2112,17 +1949,11 @@
       <c r="N27" s="8">
         <v>0</v>
       </c>
-      <c r="O27" s="8">
-        <v>0</v>
-      </c>
-      <c r="P27" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -2165,17 +1996,11 @@
       <c r="N28" s="8">
         <v>0</v>
       </c>
-      <c r="O28" s="8">
-        <v>0</v>
-      </c>
-      <c r="P28" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -2218,17 +2043,11 @@
       <c r="N29" s="8">
         <v>0</v>
       </c>
-      <c r="O29" s="8">
-        <v>0</v>
-      </c>
-      <c r="P29" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -2271,17 +2090,11 @@
       <c r="N30" s="8">
         <v>0</v>
       </c>
-      <c r="O30" s="8">
-        <v>0</v>
-      </c>
-      <c r="P30" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
@@ -2324,17 +2137,11 @@
       <c r="N31" s="8">
         <v>0</v>
       </c>
-      <c r="O31" s="8">
-        <v>0</v>
-      </c>
-      <c r="P31" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
@@ -2377,17 +2184,11 @@
       <c r="N32" s="8">
         <v>0</v>
       </c>
-      <c r="O32" s="8">
-        <v>0</v>
-      </c>
-      <c r="P32" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>31</v>
       </c>
@@ -2430,13 +2231,7 @@
       <c r="N33" s="9">
         <v>0</v>
       </c>
-      <c r="O33" s="9">
-        <v>0</v>
-      </c>
-      <c r="P33" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="11">
+      <c r="O33" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>